<commit_message>
Tests: updated the tests
</commit_message>
<xml_diff>
--- a/input_test/HMP1489_r1_t0_test_gibbs.xlsx
+++ b/input_test/HMP1489_r1_t0_test_gibbs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,396 +32,399 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="130">
-  <si>
-    <t xml:space="preserve">General Reaction and Sampling Platform (GRASP)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HMP1489_r1_t0_promiscuous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sampling mode (ORACLE, rejection, rejectionSMC, SMC, MCMC-SMC)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ORACLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLP solver (NLOPT, OPTI, FMINCON (default))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FMINCON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of exp. conditions (excluding reference state)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of model structures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of particles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parallel mode (ON = 1; OFF = 0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of cores (ignored if Parallel mode disabled)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentile of alive particles for SMC (e.g., 20, 50, etc.) (only needed for rejectionSMC, SMC, MCMC-SMC)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compute robust fluxes (ON = 1; OFF = 0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compute thermodynamics (ON = 1; OFF = 0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inicial tolerance (OPTIONAL)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Final tolerance (in the case of ORACLE, set to 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rxn ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accoa_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sam_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pterin1_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">trp_v</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fivehtp_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">trp_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">srtn_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nactsertn_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meltn_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tryptm_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nactryptm_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">coa_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sah_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pterin2_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nactryptm_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meltn_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">trp_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TPH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DDC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AANAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASMT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DDC_tryptm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AANAT_tryptm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IN_trp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_trp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_meltn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_nactryptm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metabolite name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">balanced?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">active?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fixed?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acetyl-coa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S-adenosyl-methionine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tetrahydropterin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tryptophan produced by the cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5-hydroxytryptophan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tryptophan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serotonin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N-acetylserotonin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">melatonin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tryptamine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N-acetyltryptamine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">coa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S-adenosyl-homocysteine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pterin-4a-carbinolamin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N-acetyltryptamine external</t>
-  </si>
-  <si>
-    <t xml:space="preserve">melatonin external</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tryptophan external</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">transportRxn?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">modelled?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isoenzymes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tryptophan hydroxylase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tryptophan decarboxylase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aralkylamine N-acetyltransferase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">acetylserotonin methyltransferase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">production of tryptophan by the cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exchange tryptophan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exchange melatonin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exchange n-acetyltryptamin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">met</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rxn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">∆Gr'_min (kJ/mol)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">∆Gr'_max (kJ/mol)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">min (M)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">max (M)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fluxes (umol/gCDW/h)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vref_mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vref_std</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vexp1_mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vexp1_std</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enzyme/rxn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBo10_LB2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBo10_meas2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBo10_UB2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBo10_LB2 (M)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBo10_UB2 (M)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kinetic mechanism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">substrate_order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">promiscuous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inhibitors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activators</t>
-  </si>
-  <si>
-    <t xml:space="preserve">negative effector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">positive effector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allosteric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subunits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">substrateInhibOrderedBiBi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pterin1_c trp_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fivehtp_c pterin2_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">putative homotetramer (metacyc). From pdb, might actually be a monomer. Tryptophan is substate inhibitor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UniUniPromiscuous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fivehtp_c trp_c </t>
-  </si>
-  <si>
-    <t xml:space="preserve">srtn_c tryptm_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DDC DDC_tryptm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homodimer (metacyc), inhib by serotonin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AANATCompInhibIndep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accoa_c srtn_c accoa_c tryptm_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nactsertn_c nactryptm_c coa_c coa_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AANAT AANAT_tryptm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serotonin N-acetyltransferase is a monomeric enzyme (metacyc)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">randomBiBiCompInhib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sam_c nactsertn_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meltn_c sah_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASMT has a C-terminal domain similar to other SAM-dependent O-methyltransferases, and an N-terminal domain which intertwines with another monomer to form the physiologically active dimer  (metacyc); inhib by melatonin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fivehtp_c trp_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serotonin N-acetyltransferase is a monomeric enzyme (metacyc); inhib by melatonin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">massAction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modeled as mass action</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="131">
+  <si>
+    <t>General Reaction and Sampling Platform (GRASP)</t>
+  </si>
+  <si>
+    <t>Model name</t>
+  </si>
+  <si>
+    <t>HMP1489_r1_t0_promiscuous</t>
+  </si>
+  <si>
+    <t>Sampling mode (ORACLE, rejection, rejectionSMC, SMC, MCMC-SMC)</t>
+  </si>
+  <si>
+    <t>ORACLE</t>
+  </si>
+  <si>
+    <t>NLP solver (NLOPT, OPTI, FMINCON (default))</t>
+  </si>
+  <si>
+    <t>FMINCON</t>
+  </si>
+  <si>
+    <t>Number of exp. conditions (excluding reference state)</t>
+  </si>
+  <si>
+    <t>Number of model structures</t>
+  </si>
+  <si>
+    <t>Number of particles</t>
+  </si>
+  <si>
+    <t>Parallel mode (ON = 1; OFF = 0)</t>
+  </si>
+  <si>
+    <t>Number of cores (ignored if Parallel mode disabled)</t>
+  </si>
+  <si>
+    <t>Percentile of alive particles for SMC (e.g., 20, 50, etc.) (only needed for rejectionSMC, SMC, MCMC-SMC)</t>
+  </si>
+  <si>
+    <t>Compute robust fluxes (ON = 1; OFF = 0)</t>
+  </si>
+  <si>
+    <t>Compute thermodynamics (ON = 1; OFF = 0)</t>
+  </si>
+  <si>
+    <t>Inicial tolerance (OPTIONAL)</t>
+  </si>
+  <si>
+    <t>Final tolerance (in the case of ORACLE, set to 1)</t>
+  </si>
+  <si>
+    <t>rxn ID</t>
+  </si>
+  <si>
+    <t>accoa_c</t>
+  </si>
+  <si>
+    <t>sam_c</t>
+  </si>
+  <si>
+    <t>pterin1_c</t>
+  </si>
+  <si>
+    <t>trp_v</t>
+  </si>
+  <si>
+    <t>fivehtp_c</t>
+  </si>
+  <si>
+    <t>trp_c</t>
+  </si>
+  <si>
+    <t>srtn_c</t>
+  </si>
+  <si>
+    <t>nactsertn_c</t>
+  </si>
+  <si>
+    <t>meltn_c</t>
+  </si>
+  <si>
+    <t>tryptm_c</t>
+  </si>
+  <si>
+    <t>nactryptm_c</t>
+  </si>
+  <si>
+    <t>coa_c</t>
+  </si>
+  <si>
+    <t>sah_c</t>
+  </si>
+  <si>
+    <t>pterin2_c</t>
+  </si>
+  <si>
+    <t>nactryptm_e</t>
+  </si>
+  <si>
+    <t>meltn_e</t>
+  </si>
+  <si>
+    <t>trp_e</t>
+  </si>
+  <si>
+    <t>TPH</t>
+  </si>
+  <si>
+    <t>DDC</t>
+  </si>
+  <si>
+    <t>AANAT</t>
+  </si>
+  <si>
+    <t>ASMT</t>
+  </si>
+  <si>
+    <t>DDC_tryptm</t>
+  </si>
+  <si>
+    <t>AANAT_tryptm</t>
+  </si>
+  <si>
+    <t>IN_trp</t>
+  </si>
+  <si>
+    <t>EX_trp</t>
+  </si>
+  <si>
+    <t>EX_meltn</t>
+  </si>
+  <si>
+    <t>EX_nactryptm</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Metabolite name</t>
+  </si>
+  <si>
+    <t>balanced?</t>
+  </si>
+  <si>
+    <t>active?</t>
+  </si>
+  <si>
+    <t>fixed?</t>
+  </si>
+  <si>
+    <t>measured?</t>
+  </si>
+  <si>
+    <t>Acetyl-coa</t>
+  </si>
+  <si>
+    <t>S-adenosyl-methionine</t>
+  </si>
+  <si>
+    <t>tetrahydropterin</t>
+  </si>
+  <si>
+    <t>tryptophan produced by the cell</t>
+  </si>
+  <si>
+    <t>5-hydroxytryptophan</t>
+  </si>
+  <si>
+    <t>tryptophan</t>
+  </si>
+  <si>
+    <t>serotonin</t>
+  </si>
+  <si>
+    <t>N-acetylserotonin</t>
+  </si>
+  <si>
+    <t>melatonin</t>
+  </si>
+  <si>
+    <t>tryptamine</t>
+  </si>
+  <si>
+    <t>N-acetyltryptamine</t>
+  </si>
+  <si>
+    <t>coa</t>
+  </si>
+  <si>
+    <t>S-adenosyl-homocysteine</t>
+  </si>
+  <si>
+    <t>pterin-4a-carbinolamin</t>
+  </si>
+  <si>
+    <t>N-acetyltryptamine external</t>
+  </si>
+  <si>
+    <t>melatonin external</t>
+  </si>
+  <si>
+    <t>tryptophan external</t>
+  </si>
+  <si>
+    <t>reaction name</t>
+  </si>
+  <si>
+    <t>transportRxn?</t>
+  </si>
+  <si>
+    <t>modelled?</t>
+  </si>
+  <si>
+    <t>Isoenzymes</t>
+  </si>
+  <si>
+    <t>tryptophan hydroxylase</t>
+  </si>
+  <si>
+    <t>tryptophan decarboxylase</t>
+  </si>
+  <si>
+    <t>aralkylamine N-acetyltransferase</t>
+  </si>
+  <si>
+    <t>acetylserotonin methyltransferase</t>
+  </si>
+  <si>
+    <t>production of tryptophan by the cell</t>
+  </si>
+  <si>
+    <t>exchange tryptophan</t>
+  </si>
+  <si>
+    <t>exchange melatonin</t>
+  </si>
+  <si>
+    <t>exchange n-acetyltryptamin</t>
+  </si>
+  <si>
+    <t>met</t>
+  </si>
+  <si>
+    <t>rxn</t>
+  </si>
+  <si>
+    <t>∆Gr'_min (kJ/mol)</t>
+  </si>
+  <si>
+    <t>∆Gr'_max (kJ/mol)</t>
+  </si>
+  <si>
+    <t>min (M)</t>
+  </si>
+  <si>
+    <t>max (M)</t>
+  </si>
+  <si>
+    <t>Fluxes (umol/gCDW/h)</t>
+  </si>
+  <si>
+    <t>vref_mean</t>
+  </si>
+  <si>
+    <t>vref_std</t>
+  </si>
+  <si>
+    <t>vexp1_mean</t>
+  </si>
+  <si>
+    <t>vexp1_std</t>
+  </si>
+  <si>
+    <t>enzyme/rxn</t>
+  </si>
+  <si>
+    <t>MBo10_LB2</t>
+  </si>
+  <si>
+    <t>MBo10_meas2</t>
+  </si>
+  <si>
+    <t>MBo10_UB2</t>
+  </si>
+  <si>
+    <t>MBo10_LB2 (M)</t>
+  </si>
+  <si>
+    <t>MBo10_UB2 (M)</t>
+  </si>
+  <si>
+    <t>reaction ID</t>
+  </si>
+  <si>
+    <t>kinetic mechanism</t>
+  </si>
+  <si>
+    <t>substrate_order</t>
+  </si>
+  <si>
+    <t>product_order</t>
+  </si>
+  <si>
+    <t>promiscuous</t>
+  </si>
+  <si>
+    <t>inhibitors</t>
+  </si>
+  <si>
+    <t>activators</t>
+  </si>
+  <si>
+    <t>negative effector</t>
+  </si>
+  <si>
+    <t>positive effector</t>
+  </si>
+  <si>
+    <t>allosteric</t>
+  </si>
+  <si>
+    <t>subunits</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>substrateInhibOrderedBiBi</t>
+  </si>
+  <si>
+    <t>pterin1_c trp_c</t>
+  </si>
+  <si>
+    <t>fivehtp_c pterin2_c</t>
+  </si>
+  <si>
+    <t>putative homotetramer (metacyc). From pdb, might actually be a monomer. Tryptophan is substate inhibitor</t>
+  </si>
+  <si>
+    <t>UniUniPromiscuous</t>
+  </si>
+  <si>
+    <t>fivehtp_c trp_c </t>
+  </si>
+  <si>
+    <t>srtn_c tryptm_c</t>
+  </si>
+  <si>
+    <t>DDC DDC_tryptm</t>
+  </si>
+  <si>
+    <t>homodimer (metacyc), inhib by serotonin</t>
+  </si>
+  <si>
+    <t>AANATCompInhibIndep</t>
+  </si>
+  <si>
+    <t>accoa_c srtn_c accoa_c tryptm_c</t>
+  </si>
+  <si>
+    <t>nactsertn_c nactryptm_c coa_c coa_c</t>
+  </si>
+  <si>
+    <t>AANAT AANAT_tryptm</t>
+  </si>
+  <si>
+    <t>Serotonin N-acetyltransferase is a monomeric enzyme (metacyc)</t>
+  </si>
+  <si>
+    <t>randomBiBiCompInhib</t>
+  </si>
+  <si>
+    <t>sam_c nactsertn_c</t>
+  </si>
+  <si>
+    <t>meltn_c sah_c</t>
+  </si>
+  <si>
+    <t>ASMT has a C-terminal domain similar to other SAM-dependent O-methyltransferases, and an N-terminal domain which intertwines with another monomer to form the physiologically active dimer  (metacyc); inhib by melatonin</t>
+  </si>
+  <si>
+    <t>fivehtp_c trp_c</t>
+  </si>
+  <si>
+    <t>Serotonin N-acetyltransferase is a monomeric enzyme (metacyc); inhib by melatonin</t>
+  </si>
+  <si>
+    <t>massAction</t>
+  </si>
+  <si>
+    <t>Modeled as mass action</t>
   </si>
 </sst>
 </file>
@@ -429,7 +432,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
@@ -554,7 +557,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -601,6 +604,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -690,15 +697,15 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="68.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="70.7004048582996"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -752,7 +759,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="6" t="n">
-        <v>10000</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -813,7 +820,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -828,30 +835,30 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -908,7 +915,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -923,27 +930,27 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1089,7 +1096,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1104,27 +1111,27 @@
   </sheetPr>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1368,7 +1375,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1383,54 +1390,54 @@
   </sheetPr>
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="54.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="55.914979757085"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1438,13 +1445,13 @@
         <v>35</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>110</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>111</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>23</v>
@@ -1456,7 +1463,7 @@
         <v>4</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1464,16 +1471,16 @@
         <v>36</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C3" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="C3" s="14" t="s">
         <v>114</v>
       </c>
+      <c r="D3" s="14" t="s">
+        <v>115</v>
+      </c>
       <c r="E3" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>0</v>
@@ -1482,7 +1489,7 @@
         <v>2</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1490,16 +1497,16 @@
         <v>37</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="C4" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="C4" s="14" t="s">
         <v>119</v>
       </c>
+      <c r="D4" s="14" t="s">
+        <v>120</v>
+      </c>
       <c r="E4" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>26</v>
@@ -1511,7 +1518,7 @@
         <v>1</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1519,13 +1526,13 @@
         <v>38</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="C5" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="C5" s="14" t="s">
         <v>124</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>125</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>24</v>
@@ -1537,7 +1544,7 @@
         <v>2</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1545,16 +1552,16 @@
         <v>39</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>115</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>0</v>
@@ -1563,7 +1570,7 @@
         <v>2</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1571,16 +1578,16 @@
         <v>40</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="C7" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="C7" s="14" t="s">
         <v>119</v>
       </c>
+      <c r="D7" s="14" t="s">
+        <v>120</v>
+      </c>
       <c r="E7" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>26</v>
@@ -1592,7 +1599,7 @@
         <v>1</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1600,7 +1607,7 @@
         <v>41</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>0</v>
@@ -1614,7 +1621,7 @@
         <v>42</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>0</v>
@@ -1623,7 +1630,7 @@
         <v>1</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1631,7 +1638,7 @@
         <v>43</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>0</v>
@@ -1640,7 +1647,7 @@
         <v>1</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1648,7 +1655,7 @@
         <v>44</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>0</v>
@@ -1657,13 +1664,13 @@
         <v>1</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1678,13 +1685,13 @@
   </sheetPr>
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2306,7 +2313,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2319,18 +2326,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
         <v>45</v>
       </c>
@@ -2345,6 +2352,9 @@
       </c>
       <c r="E1" s="11" t="s">
         <v>49</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2352,7 +2362,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>0</v>
@@ -2362,6 +2372,9 @@
       </c>
       <c r="E2" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2369,7 +2382,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
@@ -2379,6 +2392,9 @@
       </c>
       <c r="E3" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2386,7 +2402,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0</v>
@@ -2397,13 +2413,16 @@
       <c r="E4" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0</v>
@@ -2413,6 +2432,9 @@
       </c>
       <c r="E5" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2420,7 +2442,7 @@
         <v>22</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1</v>
@@ -2429,6 +2451,9 @@
         <v>1</v>
       </c>
       <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2437,7 +2462,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
@@ -2448,13 +2473,16 @@
       <c r="E7" s="0" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1</v>
@@ -2464,6 +2492,9 @@
       </c>
       <c r="E8" s="0" t="n">
         <v>0</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2471,7 +2502,7 @@
         <v>25</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1</v>
@@ -2480,6 +2511,9 @@
         <v>1</v>
       </c>
       <c r="E9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2488,7 +2522,7 @@
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>1</v>
@@ -2498,6 +2532,9 @@
       </c>
       <c r="E10" s="0" t="n">
         <v>0</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2505,7 +2542,7 @@
         <v>27</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1</v>
@@ -2514,6 +2551,9 @@
         <v>1</v>
       </c>
       <c r="E11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2522,7 +2562,7 @@
         <v>28</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>1</v>
@@ -2531,6 +2571,9 @@
         <v>1</v>
       </c>
       <c r="E12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2539,7 +2582,7 @@
         <v>29</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>0</v>
@@ -2550,13 +2593,16 @@
       <c r="E13" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F13" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>0</v>
@@ -2566,6 +2612,9 @@
       </c>
       <c r="E14" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2573,7 +2622,7 @@
         <v>31</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>0</v>
@@ -2583,6 +2632,9 @@
       </c>
       <c r="E15" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2590,7 +2642,7 @@
         <v>32</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>0</v>
@@ -2600,6 +2652,9 @@
       </c>
       <c r="E16" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2607,7 +2662,7 @@
         <v>33</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>0</v>
@@ -2617,6 +2672,9 @@
       </c>
       <c r="E17" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2624,7 +2682,7 @@
         <v>34</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>0</v>
@@ -2634,12 +2692,15 @@
       </c>
       <c r="E18" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2654,13 +2715,13 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2668,16 +2729,16 @@
         <v>45</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" s="12" t="s">
         <v>70</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2685,7 +2746,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>0</v>
@@ -2699,7 +2760,7 @@
         <v>36</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
@@ -2713,7 +2774,7 @@
         <v>37</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0</v>
@@ -2727,7 +2788,7 @@
         <v>38</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0</v>
@@ -2741,7 +2802,7 @@
         <v>39</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0</v>
@@ -2755,7 +2816,7 @@
         <v>40</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>0</v>
@@ -2769,7 +2830,7 @@
         <v>41</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>0</v>
@@ -2783,7 +2844,7 @@
         <v>42</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>0</v>
@@ -2797,7 +2858,7 @@
         <v>43</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0</v>
@@ -2811,7 +2872,7 @@
         <v>44</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>0</v>
@@ -2823,7 +2884,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2838,13 +2899,13 @@
   </sheetPr>
   <dimension ref="A2:A12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2905,7 +2966,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2920,18 +2981,18 @@
   </sheetPr>
   <dimension ref="A2:A19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3022,7 +3083,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3037,18 +3098,18 @@
   </sheetPr>
   <dimension ref="A2:A19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3139,7 +3200,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3154,27 +3215,27 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3290,7 +3351,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3305,24 +3366,24 @@
   </sheetPr>
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3515,7 +3576,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>